<commit_message>
Catchall commit. Updated to_do_list, created a template for Jeremy to collect potyvirus information, modified the LY104 sequences file. For the latter, added in the sequences for newly ordered primers to put Htra1 into LY104.
</commit_message>
<xml_diff>
--- a/protease_design/potyvirus/potyvirus_proteases.xlsx
+++ b/protease_design/potyvirus/potyvirus_proteases.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="192">
   <si>
     <t>Name</t>
   </si>
@@ -597,6 +597,12 @@
   </si>
   <si>
     <t>ZYMV</t>
+  </si>
+  <si>
+    <t>SBMV</t>
+  </si>
+  <si>
+    <t>IN LAB</t>
   </si>
 </sst>
 </file>
@@ -940,8 +946,8 @@
   <dimension ref="A1:E169"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D117" sqref="D117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,37 +1467,37 @@
         <v>99</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>106</v>
       </c>
@@ -1499,50 +1505,53 @@
         <v>183</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>113</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E110" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>115</v>
       </c>
@@ -1550,12 +1559,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>117</v>
       </c>
@@ -1563,47 +1572,53 @@
         <v>174</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B122" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>126</v>
       </c>
@@ -1611,27 +1626,27 @@
         <v>186</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
         <v>131</v>
       </c>

</xml_diff>